<commit_message>
Hoan Thanh Co Chuong Trinh Cho Quan Tri Vien
</commit_message>
<xml_diff>
--- a/ThongKeCuaCoSoDuLieu.xlsx
+++ b/ThongKeCuaCoSoDuLieu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lesson\RIT\C #\Winform\TravelAgency\QuanLyCongTyDuLich\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lesson\RIT\C #\ABC\QuanLyCongTyDuLich\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9E579B-26C0-4F96-9A8C-7F8DC8D72DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995FEFDF-B19D-4C72-82E2-A75B7C7CF390}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{26AF44B8-D7A5-4443-B26F-F8CB78977FA3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
   <si>
     <t>Amazing</t>
   </si>
@@ -93,24 +93,12 @@
     <t>paris</t>
   </si>
   <si>
-    <t>Bangkok</t>
-  </si>
-  <si>
-    <t>Maria Catheral</t>
-  </si>
-  <si>
-    <t>mandalay</t>
-  </si>
-  <si>
     <t>Kalemegdan</t>
   </si>
   <si>
     <t>Jeju</t>
   </si>
   <si>
-    <t>Seol</t>
-  </si>
-  <si>
     <t>Skadarlija</t>
   </si>
   <si>
@@ -129,18 +117,12 @@
     <t>Beijing</t>
   </si>
   <si>
-    <t>Rio De Janerio</t>
-  </si>
-  <si>
     <t>Talin</t>
   </si>
   <si>
     <t>Gdansk</t>
   </si>
   <si>
-    <t>berlin</t>
-  </si>
-  <si>
     <t>Petrovaradin</t>
   </si>
   <si>
@@ -150,9 +132,6 @@
     <t>Serengeti</t>
   </si>
   <si>
-    <t>Titicaca Lake</t>
-  </si>
-  <si>
     <t>Larnaca</t>
   </si>
   <si>
@@ -163,6 +142,120 @@
   </si>
   <si>
     <t>Sharm El Sheikh</t>
+  </si>
+  <si>
+    <t>BangKok</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Titicaca</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Rio De Janeiro</t>
+  </si>
+  <si>
+    <t>Mandalay</t>
+  </si>
+  <si>
+    <t>serengeti</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Sigriswil Urban</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Kilimanjaro</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Kyoto</t>
+  </si>
+  <si>
+    <t>Obwalden</t>
+  </si>
+  <si>
+    <t>Bazaruto Island</t>
+  </si>
+  <si>
+    <t>Cusco</t>
+  </si>
+  <si>
+    <t>Jeju Island</t>
+  </si>
+  <si>
+    <t>St. Petersburg</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Labadee</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>venice</t>
+  </si>
+  <si>
+    <t>Fatucama Peninsula</t>
+  </si>
+  <si>
+    <t>Misti Volcano</t>
+  </si>
+  <si>
+    <t>Grindelwald</t>
+  </si>
+  <si>
+    <t>Isetwald</t>
+  </si>
+  <si>
+    <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>Maria Cathedral</t>
+  </si>
+  <si>
+    <t>@@@@</t>
+  </si>
+  <si>
+    <t>Lviv</t>
+  </si>
+  <si>
+    <t>Odessa</t>
+  </si>
+  <si>
+    <t>Oku Mountain</t>
+  </si>
+  <si>
+    <t>Inhambane</t>
+  </si>
+  <si>
+    <t>Zan+N9:Q9zibar</t>
+  </si>
+  <si>
+    <t>Maputo Church</t>
+  </si>
+  <si>
+    <t>Venice</t>
   </si>
 </sst>
 </file>
@@ -198,8 +291,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,51 +608,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C77655-8433-4607-9250-1002B46880E1}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="14" max="14" width="18.5703125" customWidth="1"/>
     <col min="15" max="15" width="18.140625" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>130</v>
+        <v>6</v>
       </c>
       <c r="E1">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="F1">
-        <v>20</v>
+        <v>150</v>
+      </c>
+      <c r="G1">
+        <v>320</v>
+      </c>
+      <c r="H1">
+        <v>640</v>
       </c>
       <c r="N1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>170</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>373</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>135</v>
+      </c>
+      <c r="G2">
+        <v>453</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
@@ -566,292 +698,688 @@
       <c r="O2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>250</v>
+      </c>
+      <c r="G3">
+        <v>159</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>70</v>
+        <v>483</v>
       </c>
       <c r="F4">
+        <v>865</v>
+      </c>
+      <c r="G4">
+        <v>240</v>
+      </c>
+      <c r="H4">
+        <v>230</v>
+      </c>
+      <c r="N4" t="s">
         <v>30</v>
       </c>
-      <c r="N4" t="s">
-        <v>40</v>
-      </c>
       <c r="O4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>461</v>
+      </c>
+      <c r="F5">
         <v>165</v>
       </c>
-      <c r="E5">
-        <v>85</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
+      <c r="G5">
+        <v>250</v>
+      </c>
+      <c r="H5">
+        <v>290</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="O5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="P5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>180</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>100</v>
       </c>
       <c r="F6">
-        <v>40</v>
+        <v>135</v>
+      </c>
+      <c r="G6">
+        <v>450</v>
+      </c>
+      <c r="H6">
+        <v>260</v>
+      </c>
+      <c r="I6">
+        <v>265</v>
+      </c>
+      <c r="J6">
+        <v>510</v>
       </c>
       <c r="N6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" t="s">
+        <v>71</v>
+      </c>
+      <c r="S6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>195</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>95</v>
+        <v>146</v>
+      </c>
+      <c r="F7">
+        <v>650</v>
+      </c>
+      <c r="G7">
+        <v>230</v>
+      </c>
+      <c r="H7">
+        <v>340</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="O7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>70</v>
+        <v>341</v>
+      </c>
+      <c r="F8">
+        <v>220</v>
+      </c>
+      <c r="G8">
+        <v>455</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="O8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>185</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>85</v>
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>145</v>
+      </c>
+      <c r="G9">
+        <v>310</v>
+      </c>
+      <c r="H9">
+        <v>290</v>
+      </c>
+      <c r="I9" s="1">
+        <v>462</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="O9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>80</v>
+        <v>715</v>
+      </c>
+      <c r="F10">
+        <v>410</v>
+      </c>
+      <c r="G10">
+        <v>320</v>
+      </c>
+      <c r="H10">
+        <v>260</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="O10" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>160</v>
+      </c>
+      <c r="F11">
+        <v>245</v>
+      </c>
+      <c r="G11">
+        <v>510</v>
+      </c>
+      <c r="H11">
+        <v>160</v>
+      </c>
+      <c r="I11">
+        <v>340</v>
       </c>
       <c r="N11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="O11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>68</v>
+      </c>
+      <c r="R11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>100</v>
+        <v>731</v>
+      </c>
+      <c r="F12">
+        <v>120</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="O12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>70</v>
+        <v>415</v>
+      </c>
+      <c r="F13">
+        <v>310</v>
+      </c>
+      <c r="G13">
+        <v>410</v>
+      </c>
+      <c r="H13">
+        <v>190</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="O13" t="s">
+        <v>57</v>
+      </c>
+      <c r="P13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>60</v>
+        <v>420</v>
+      </c>
+      <c r="F14">
+        <v>160</v>
+      </c>
+      <c r="G14">
+        <v>270</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="O14" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>300</v>
+      </c>
+      <c r="F15">
         <v>150</v>
       </c>
-      <c r="E15">
-        <v>80</v>
+      <c r="G15">
+        <v>525</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="O15" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>50</v>
+        <v>210</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>400</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>210</v>
+        <v>235</v>
+      </c>
+      <c r="F17">
+        <v>315</v>
+      </c>
+      <c r="G17">
+        <v>280</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="N17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="O17" t="s">
+        <v>48</v>
+      </c>
+      <c r="P17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>200</v>
+        <v>9</v>
       </c>
       <c r="E18">
-        <v>150</v>
+        <v>650</v>
+      </c>
+      <c r="F18">
+        <v>490</v>
+      </c>
+      <c r="G18">
+        <v>665</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O18" t="s">
+        <v>60</v>
+      </c>
+      <c r="P18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>500</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>410</v>
+        <v>760</v>
+      </c>
+      <c r="F19">
+        <v>290</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="O19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>420</v>
+        <v>6</v>
       </c>
       <c r="E20">
-        <v>160</v>
+        <v>462</v>
+      </c>
+      <c r="F20">
+        <v>135</v>
+      </c>
+      <c r="G20">
+        <v>135</v>
       </c>
       <c r="N20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="O20" t="s">
+        <v>26</v>
+      </c>
+      <c r="P20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>860</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>230</v>
+        <v>352</v>
+      </c>
+      <c r="F21">
+        <v>329</v>
+      </c>
+      <c r="G21">
+        <v>240</v>
+      </c>
+      <c r="H21">
+        <v>190</v>
       </c>
       <c r="N21" t="s">
         <v>21</v>
+      </c>
+      <c r="O21" t="s">
+        <v>24</v>
+      </c>
+      <c r="P21" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>